<commit_message>
xlxs for freelancer, k=0.2, k=4 xlxs for guru
</commit_message>
<xml_diff>
--- a/results/real_data_freelancer_0.2_opt_constrained/k=0.2/CSG/dataset_05/results_excel_26-9-22_freelancer_constrained_1_.xlsx
+++ b/results/real_data_freelancer_0.2_opt_constrained/k=0.2/CSG/dataset_05/results_excel_26-9-22_freelancer_constrained_1_.xlsx
@@ -1,20 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Konstantina\Desktop\HDrop20-Master-Thesis-Experiments\results\real_data_freelancer_0.2_opt_constrained\k=0.2\CSG\dataset_05\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F628C2A1-6FE6-4511-A82D-0E317D85F860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>dataset</t>
   </si>
@@ -122,13 +141,25 @@
   </si>
   <si>
     <t>Official_Experiment_CSG_dataset_05_instance_10_9_exec</t>
+  </si>
+  <si>
+    <t>Average of SW(S*)/SW(OPT)</t>
+  </si>
+  <si>
+    <t>Average of SC(S*)/SC(OPT)</t>
+  </si>
+  <si>
+    <t>Worst of SW(S*)/SW(OPT)</t>
+  </si>
+  <si>
+    <t>Worst of SC(S*)/SC(OPT)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +173,24 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="161"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="161"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -180,22 +229,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Θέμα του Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -237,7 +298,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -269,9 +330,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -303,6 +382,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -478,14 +575,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:B17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -562,7 +661,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -603,7 +702,7 @@
         <v>0.2</v>
       </c>
       <c r="N2">
-        <v>0.9587301587301588</v>
+        <v>0.95873015873015877</v>
       </c>
       <c r="O2">
         <v>380</v>
@@ -612,13 +711,13 @@
         <v>65</v>
       </c>
       <c r="Q2">
-        <v>1.765783982824794</v>
+        <v>1.7657839828247941</v>
       </c>
       <c r="R2">
-        <v>200.2240411163884</v>
+        <v>200.22404111638841</v>
       </c>
       <c r="S2">
-        <v>5.846153846153846</v>
+        <v>5.8461538461538458</v>
       </c>
       <c r="T2">
         <v>7.04</v>
@@ -627,7 +726,7 @@
         <v>1.951608170169951</v>
       </c>
       <c r="V2">
-        <v>204.4195914915024</v>
+        <v>204.41959149150239</v>
       </c>
       <c r="W2">
         <v>429</v>
@@ -642,7 +741,7 @@
         <v>1.03125</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -722,7 +821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -772,10 +871,10 @@
         <v>5</v>
       </c>
       <c r="Q4">
-        <v>2.785011242238338</v>
+        <v>2.7850112422383382</v>
       </c>
       <c r="R4">
-        <v>62.07494378880831</v>
+        <v>62.074943788808312</v>
       </c>
       <c r="S4">
         <v>16.2</v>
@@ -784,10 +883,10 @@
         <v>16.2</v>
       </c>
       <c r="U4">
-        <v>2.785011242238338</v>
+        <v>2.7850112422383382</v>
       </c>
       <c r="V4">
-        <v>62.07494378880831</v>
+        <v>62.074943788808312</v>
       </c>
       <c r="W4">
         <v>516</v>
@@ -802,7 +901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -852,22 +951,22 @@
         <v>43</v>
       </c>
       <c r="Q5">
-        <v>1.81852971029266</v>
+        <v>1.8185297102926601</v>
       </c>
       <c r="R5">
-        <v>143.8032224574156</v>
+        <v>143.80322245741559</v>
       </c>
       <c r="S5">
-        <v>6.162790697674419</v>
+        <v>6.1627906976744189</v>
       </c>
       <c r="T5">
-        <v>6.162790697674419</v>
+        <v>6.1627906976744189</v>
       </c>
       <c r="U5">
-        <v>1.81852971029266</v>
+        <v>1.8185297102926601</v>
       </c>
       <c r="V5">
-        <v>143.8032224574156</v>
+        <v>143.80322245741559</v>
       </c>
       <c r="W5">
         <v>342</v>
@@ -882,7 +981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -932,10 +1031,10 @@
         <v>48</v>
       </c>
       <c r="Q6">
-        <v>2.698280409506405</v>
+        <v>2.6982804095064048</v>
       </c>
       <c r="R6">
-        <v>535.4825403436926</v>
+        <v>535.48254034369256</v>
       </c>
       <c r="S6">
         <v>14.85416666666667</v>
@@ -944,10 +1043,10 @@
         <v>14.85416666666667</v>
       </c>
       <c r="U6">
-        <v>2.698280409506405</v>
+        <v>2.6982804095064048</v>
       </c>
       <c r="V6">
-        <v>535.4825403436926</v>
+        <v>535.48254034369256</v>
       </c>
       <c r="W6">
         <v>830</v>
@@ -962,7 +1061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1003,7 +1102,7 @@
         <v>0.2</v>
       </c>
       <c r="N7">
-        <v>0.979381443298969</v>
+        <v>0.97938144329896903</v>
       </c>
       <c r="O7">
         <v>247</v>
@@ -1015,13 +1114,13 @@
         <v>1.539096423075855</v>
       </c>
       <c r="R7">
-        <v>112.4278895769797</v>
+        <v>112.42788957697969</v>
       </c>
       <c r="S7">
-        <v>4.660377358490566</v>
+        <v>4.6603773584905657</v>
       </c>
       <c r="T7">
-        <v>5.418604651162791</v>
+        <v>5.4186046511627914</v>
       </c>
       <c r="U7">
         <v>1.689838337872138</v>
@@ -1042,7 +1141,7 @@
         <v>1.008163265306123</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1083,7 +1182,7 @@
         <v>0.2</v>
       </c>
       <c r="N8">
-        <v>0.9478260869565217</v>
+        <v>0.94782608695652171</v>
       </c>
       <c r="O8">
         <v>140</v>
@@ -1095,19 +1194,19 @@
         <v>1.722766597741104</v>
       </c>
       <c r="R8">
-        <v>71.9308350564724</v>
+        <v>71.930835056472404</v>
       </c>
       <c r="S8">
         <v>5.6</v>
       </c>
       <c r="T8">
-        <v>8.266666666666667</v>
+        <v>8.2666666666666675</v>
       </c>
       <c r="U8">
         <v>2.112231364502827</v>
       </c>
       <c r="V8">
-        <v>77.31652953245759</v>
+        <v>77.316529532457594</v>
       </c>
       <c r="W8">
         <v>292</v>
@@ -1122,7 +1221,7 @@
         <v>1.020979020979021</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1175,19 +1274,19 @@
         <v>2.819439021591386</v>
       </c>
       <c r="R9">
-        <v>556.7641220715703</v>
+        <v>556.76412207157034</v>
       </c>
       <c r="S9">
-        <v>16.76744186046512</v>
+        <v>16.767441860465119</v>
       </c>
       <c r="T9">
-        <v>16.76744186046512</v>
+        <v>16.767441860465119</v>
       </c>
       <c r="U9">
         <v>2.819439021591386</v>
       </c>
       <c r="V9">
-        <v>556.7641220715703</v>
+        <v>556.76412207157034</v>
       </c>
       <c r="W9">
         <v>885</v>
@@ -1202,7 +1301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1255,7 +1354,7 @@
         <v>2.456735772821304</v>
       </c>
       <c r="R10">
-        <v>394.0766829045774</v>
+        <v>394.07668290457741</v>
       </c>
       <c r="S10">
         <v>11.66666666666667</v>
@@ -1282,7 +1381,7 @@
         <v>1.003134796238244</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1323,7 +1422,7 @@
         <v>0.15</v>
       </c>
       <c r="N11">
-        <v>0.7551020408163265</v>
+        <v>0.75510204081632648</v>
       </c>
       <c r="O11">
         <v>136</v>
@@ -1332,7 +1431,7 @@
         <v>87</v>
       </c>
       <c r="Q11">
-        <v>0.4467467670814683</v>
+        <v>0.44674676708146832</v>
       </c>
       <c r="R11">
         <v>10.13303126391226</v>
@@ -1347,7 +1446,7 @@
         <v>1.547562508716013</v>
       </c>
       <c r="V11">
-        <v>21.52437491283987</v>
+        <v>21.524374912839871</v>
       </c>
       <c r="W11">
         <v>492</v>
@@ -1359,10 +1458,53 @@
         <v>480</v>
       </c>
       <c r="Z11">
-        <v>1.025</v>
+        <v>1.0249999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="J12" s="3">
+        <f>AVERAGE(J2:J11)</f>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="2">
+        <f>AVERAGE(N2:N11)</f>
+        <v>0.96371334798019759</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="2">
+        <f>AVERAGE(Z2:Z11)</f>
+        <v>1.0088527082523389</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="2">
+        <f>MIN(N2:N11)</f>
+        <v>0.75510204081632648</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="2">
+        <f>MAX(Z2:Z11)</f>
+        <v>1.03125</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>